<commit_message>
Replaced the file with Workflow updates
</commit_message>
<xml_diff>
--- a/assets/other/Claims-V1.xlsx
+++ b/assets/other/Claims-V1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08AF4FFB-BDB8-4DD5-ADBC-CC9E31186FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7E6CE61-B138-452D-9E8F-6FFA7C709972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1013,13 +1013,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1357,7 +1356,7 @@
   <dimension ref="A1:G205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="E205" sqref="E205"/>
+      <selection activeCell="D203" sqref="D203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2549,42 +2548,42 @@
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="5" t="s">
+      <c r="A59" t="s">
         <v>82</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" t="s">
         <v>97</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" t="s">
         <v>103</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" t="s">
         <v>99</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E59" t="s">
         <v>100</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F59" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="5" t="s">
+      <c r="A60" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" t="s">
         <v>97</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" t="s">
         <v>104</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" t="s">
         <v>99</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E60" t="s">
         <v>100</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4222,7 +4221,7 @@
         <v>213</v>
       </c>
       <c r="F142" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -4242,7 +4241,7 @@
         <v>213</v>
       </c>
       <c r="F143" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -4262,7 +4261,7 @@
         <v>213</v>
       </c>
       <c r="F144" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -4282,7 +4281,7 @@
         <v>213</v>
       </c>
       <c r="F145" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:6">

</xml_diff>